<commit_message>
CIIP Model and CDM manual updates
</commit_message>
<xml_diff>
--- a/docs/CDM-manual/tables/wave_pars.xlsx
+++ b/docs/CDM-manual/tables/wave_pars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\00065525\Github\CDM\docs\CDM-manual\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F59948-1164-4905-B57E-13FC481D2BEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BD64C30-C7E3-4A88-8FDA-1594914BBF39}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5400" yWindow="2835" windowWidth="21600" windowHeight="11505" xr2:uid="{DECC0CF8-79EF-43B2-948C-02F9DA64B271}"/>
+    <workbookView xWindow="5055" yWindow="2490" windowWidth="21600" windowHeight="11505" xr2:uid="{DECC0CF8-79EF-43B2-948C-02F9DA64B271}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -141,21 +141,6 @@
   </si>
   <si>
     <r>
-      <t>0.01-1</t>
-    </r>
-    <r>
-      <rPr>
-        <vertAlign val="superscript"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> $^d, e$</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t>0.02-0.25$^{</t>
     </r>
     <r>
@@ -167,6 +152,21 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve"> b,c}$</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>0.01-1</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> $^{d, e}$</t>
     </r>
   </si>
 </sst>
@@ -599,7 +599,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -658,7 +658,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="4">
         <v>0.05</v>
@@ -698,7 +698,7 @@
         <v>12</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F5" s="4">
         <v>0.2</v>

</xml_diff>